<commit_message>
edits to scripts, new files and output
</commit_message>
<xml_diff>
--- a/Frayling_et_al/data_files/2014_03_02_interaction_checks_epiGPU_ARW+MNW_v2_JEP.xlsx
+++ b/Frayling_et_al/data_files/2014_03_02_interaction_checks_epiGPU_ARW+MNW_v2_JEP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-41020" yWindow="-460" windowWidth="37860" windowHeight="17360" tabRatio="500"/>
+    <workbookView xWindow="-50620" yWindow="-2360" windowWidth="26380" windowHeight="21560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA FORMATTED" sheetId="5" r:id="rId1"/>
@@ -1115,8 +1115,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="381">
+  <cellStyleXfs count="397">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1886,7 +1902,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="381">
+  <cellStyles count="397">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2077,6 +2093,14 @@
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2267,6 +2291,14 @@
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2603,8 +2635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0"/>

</xml_diff>